<commit_message>
update concept and data
</commit_message>
<xml_diff>
--- a/excel/fupan_stocks_non_main.xlsx
+++ b/excel/fupan_stocks_non_main.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CJ7"/>
+  <dimension ref="A1:CK7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -874,6 +874,11 @@
           <t>2025年05月16日</t>
         </is>
       </c>
+      <c r="CK1" s="1" t="inlineStr">
+        <is>
+          <t>2025年05月19日</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -1107,6 +1112,11 @@
       <c r="CJ2" t="inlineStr">
         <is>
           <t>301089.SZ; 拓新药业; 0;  14:19:54; 2天2板; 37.78;  14:19:54; 20.0%; 2; 麦角硫因+合成生物+原料药</t>
+        </is>
+      </c>
+      <c r="CK2" t="inlineStr">
+        <is>
+          <t>300963.SZ; 中洲特材; 0;  11:20:21; 2天2板; 29.59;  11:20:21; 20.0%; 2; 核电+海工装备+焊材</t>
         </is>
       </c>
     </row>
@@ -1421,7 +1431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CJ532"/>
+  <dimension ref="A1:CK532"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1863,6 +1873,11 @@
       <c r="CJ1" s="1" t="inlineStr">
         <is>
           <t>2025年05月16日</t>
+        </is>
+      </c>
+      <c r="CK1" s="1" t="inlineStr">
+        <is>
+          <t>2025年05月19日</t>
         </is>
       </c>
     </row>
@@ -7242,7 +7257,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CJ11"/>
+  <dimension ref="A1:CK11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7686,6 +7701,11 @@
           <t>2025年05月16日</t>
         </is>
       </c>
+      <c r="CK1" s="1" t="inlineStr">
+        <is>
+          <t>2025年05月19日</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -8101,6 +8121,11 @@
           <t>300258.SZ; 精锻科技; 1;  09:57:00; 16.82; 曾涨停; 12.3%; 0.19H;  09:57:00</t>
         </is>
       </c>
+      <c r="CK2" t="inlineStr">
+        <is>
+          <t>300609.SZ; 汇纳科技; 1;  09:39:33; 33.79; 曾涨停; 15.0%; 0.06H;  09:39:33</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -8454,6 +8479,11 @@
       <c r="CJ3" t="inlineStr">
         <is>
           <t>300328.SZ; 宜安科技; 1;  10:15:39; 12.79; 曾涨停; 14.4%; 0.14H;  10:15:39</t>
+        </is>
+      </c>
+      <c r="CK3" t="inlineStr">
+        <is>
+          <t>300210.SZ; 森远股份; 1;  10:58:18; 11.19; 曾涨停; 15.4%; 1.20H;  10:58:18</t>
         </is>
       </c>
     </row>
@@ -9228,7 +9258,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CJ30"/>
+  <dimension ref="A1:CK30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9672,6 +9702,11 @@
           <t>2025年05月16日</t>
         </is>
       </c>
+      <c r="CK1" s="1" t="inlineStr">
+        <is>
+          <t>2025年05月19日</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -10107,6 +10142,11 @@
           <t>301488.SZ; 豪恩汽电; 0;  10:36:09; 首板涨停; 73.8;  10:36:09; 20.0%; 1; 自动紧急制动AEB+人形机器人+智能驾驶</t>
         </is>
       </c>
+      <c r="CK2" t="inlineStr">
+        <is>
+          <t>300489.SZ; 光智科技; 1;  09:37:39; 首板涨停; 53.42;  09:25:00; 20.0%; 1; 拟并购先导电科+红外光学</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -10527,6 +10567,11 @@
           <t>301260.SZ; 格力博; 0;  11:24:24; 首板涨停; 20.5;  11:24:24; 20.0%; 1; 机器人+新能源园林机械+中越美制造基地+外销</t>
         </is>
       </c>
+      <c r="CK3" t="inlineStr">
+        <is>
+          <t>300069.SZ; 金利华电; 0;  09:57:51; 首板涨停; 19.5;  09:57:51; 20.0%; 1; 拟购买海德利森100%股权+电网设备</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -10917,6 +10962,11 @@
           <t>300963.SZ; 中洲特材; 13;  14:35:18; 首板涨停; 24.66;  09:41:57; 20.0%; 1; 核电+海工装备+焊材</t>
         </is>
       </c>
+      <c r="CK4" t="inlineStr">
+        <is>
+          <t>300631.SZ; 久吾高科; 1;  11:15:03; 首板涨停; 24.58;  10:09:27; 20.0%; 1; 一季报增长+盐湖提锂+膜技术</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -11267,6 +11317,11 @@
           <t>837023.BJ; 芭薇股份; 2;  13:00:00; 首板涨停; 35.39;  10:15:09; 30.0%; 1; 化妆品+合成生物+海外拓展</t>
         </is>
       </c>
+      <c r="CK5" t="inlineStr">
+        <is>
+          <t>835174.BJ; 五新隧装; 2;  11:29:42; 首板涨停; 42.84;  10:56:42; 30.0%; 1; 重大资产重组+基建+一带一路</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -11587,6 +11642,11 @@
           <t>301089.SZ; 拓新药业; 0;  13:22:21; 首板涨停; 31.48;  13:22:21; 20.0%; 1; 麦角硫因+合成生物+原料药</t>
         </is>
       </c>
+      <c r="CK6" t="inlineStr">
+        <is>
+          <t>301335.SZ; 天元宠物; 1;  14:04:21; 首板涨停; 37.08;  13:28:51; 20.0%; 1; 资产重组+宠物经济+跨境电商</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -11857,6 +11917,11 @@
           <t>300886.SZ; 华业香料; 0;  13:23:39; 首板涨停; 27.16;  13:23:39; 20.0%; 1; 香料+外销+一季报增长+产能释放</t>
         </is>
       </c>
+      <c r="CK7" t="inlineStr">
+        <is>
+          <t>688336.SH; 三生国健; 0;  14:20:17; 首板涨停; 32.81;  14:20:17; 20.0%; 1; 创新药+自免+重组蛋白</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -12092,6 +12157,11 @@
           <t>300132.SZ; 青松股份; 3;  14:40:30; 首板涨停; 6.4;  14:23:54; 20.1%; 1; 化妆品+美容护理+合成生物</t>
         </is>
       </c>
+      <c r="CK8" t="inlineStr">
+        <is>
+          <t>301459.SZ; 丰茂股份; 1;  14:22:54; 首板涨停; 65.75;  13:00:00; 20.0%; 1; 汽车零部件+人形机器人+橡胶</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -12265,6 +12335,11 @@
       <c r="CD9" t="inlineStr">
         <is>
           <t>873169.BJ; 七丰精工; 2;  13:44:50; 首板涨停; 27.39;  10:21:27; 17.5%; 1; 航空航天+轨道交通+一季报增长</t>
+        </is>
+      </c>
+      <c r="CK9" t="inlineStr">
+        <is>
+          <t>300927.SZ; 江天化学; 0;  14:53:21; 首板涨停; 36.83;  14:53:21; 20.0%; 1; 甲醛+可用于生产季戊四醇+国企</t>
         </is>
       </c>
     </row>
@@ -13189,7 +13264,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CJ178"/>
+  <dimension ref="A1:CK178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13633,6 +13708,11 @@
           <t>2025年05月16日</t>
         </is>
       </c>
+      <c r="CK1" s="1" t="inlineStr">
+        <is>
+          <t>2025年05月19日</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -14048,6 +14128,11 @@
           <t>300258.SZ; 精锻科技; 2.4%; 15.0%; 16.82; 12.3%; 价升量涨||阳线||放量</t>
         </is>
       </c>
+      <c r="CK2" t="inlineStr">
+        <is>
+          <t>871396.BJ; 常辅股份; 5.3%; 28.8%; 49.6; 22.0%; 价升量涨||强中选强||阳线</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -14428,6 +14513,11 @@
           <t>300328.SZ; 宜安科技; 1.8%; 16.5%; 12.79; 14.4%; 价升量涨||阳线||放量</t>
         </is>
       </c>
+      <c r="CK3" t="inlineStr">
+        <is>
+          <t>300963.SZ; 中洲特材; 4.9%; 26.2%; 29.59; 20.0%; 强中选强||阳线||放量</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -14768,6 +14858,11 @@
           <t>301260.SZ; 格力博; 1.6%; 22.0%; 20.5; 20.0%; 价升量涨||阳线||放量</t>
         </is>
       </c>
+      <c r="CK4" t="inlineStr">
+        <is>
+          <t>836077.BJ; 吉林碳谷; 3.6%; 19.6%; 16.69; 15.3%; 价升量涨||强中选强||阳线</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -15071,6 +15166,11 @@
       <c r="CJ5" t="inlineStr">
         <is>
           <t>301283.SZ; 聚胶股份; 1.0%; 12.9%; 35.16; 11.8%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
+      <c r="CK5" t="inlineStr">
+        <is>
+          <t>300004.SZ; 南风股份; 0.1%; 12.0%; 9.96; 11.9%; 价升量涨||强中选强||阳线</t>
         </is>
       </c>
     </row>
@@ -18890,7 +18990,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CJ21"/>
+  <dimension ref="A1:CK21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19334,6 +19434,11 @@
           <t>2025年05月16日</t>
         </is>
       </c>
+      <c r="CK1" s="1" t="inlineStr">
+        <is>
+          <t>2025年05月19日</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -19774,6 +19879,11 @@
           <t>300963.SZ; 中洲特材; 24.66; 20.0%; 126793.0; 26</t>
         </is>
       </c>
+      <c r="CK2" t="inlineStr">
+        <is>
+          <t>301316.SZ; 慧博云通; nan; nan%; 274162.0; 12</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -20214,6 +20324,11 @@
           <t>301089.SZ; 拓新药业; 37.78; 20.0%; 117171.5; 31</t>
         </is>
       </c>
+      <c r="CK3" t="inlineStr">
+        <is>
+          <t>300963.SZ; 中洲特材; 29.59; 20.0%; 253667.5; 15</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -20654,6 +20769,11 @@
           <t>300607.SZ; 拓斯达; 37.8; -2.8%; 92736.0; 43</t>
         </is>
       </c>
+      <c r="CK4" t="inlineStr">
+        <is>
+          <t>300927.SZ; 江天化学; 36.83; 20.0%; 191644.0; 25</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -21094,6 +21214,11 @@
           <t>302132.SZ; 中航成飞; 86.08; -1.1%; 80580.5; 49</t>
         </is>
       </c>
+      <c r="CK5" t="inlineStr">
+        <is>
+          <t>300879.SZ; 大叶股份; 53.9; 13.5%; 171894.0; 31</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -21534,6 +21659,11 @@
           <t>301488.SZ; 豪恩汽电; 73.8; 20.0%; 77782.0; 52</t>
         </is>
       </c>
+      <c r="CK6" t="inlineStr">
+        <is>
+          <t>301595.SZ; 太力科技; 54.3; 218.5%; 146135.5; 50</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -21974,6 +22104,11 @@
           <t>300879.SZ; 大叶股份; 47.5; -5.0%; 71136.5; 56</t>
         </is>
       </c>
+      <c r="CK7" t="inlineStr">
+        <is>
+          <t>300489.SZ; 光智科技; 53.42; 20.0%; 122262.0; 65</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -22414,6 +22549,11 @@
           <t>301260.SZ; 格力博; 20.5; 20.0%; 70583.5; 58</t>
         </is>
       </c>
+      <c r="CK8" t="inlineStr">
+        <is>
+          <t>301335.SZ; 天元宠物; 37.08; 20.0%; 122058.0; 67</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -22854,6 +22994,11 @@
           <t>300946.SZ; 恒而达; 80; 11.1%; 60554.5; 70</t>
         </is>
       </c>
+      <c r="CK9" t="inlineStr">
+        <is>
+          <t>302132.SZ; 中航成飞; 87.2; 1.3%; 107994.0; 74</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -23294,6 +23439,11 @@
           <t>300100.SZ; 双林股份; 52.7; -4.0%; 55460.5; 77</t>
         </is>
       </c>
+      <c r="CK10" t="inlineStr">
+        <is>
+          <t>300047.SZ; 天源迪科; 16.92; 5.2%; 97197.5; 86</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -23734,6 +23884,11 @@
           <t>301636.SZ; 泽润新能; 65.96; 99.5%; 54936.0; 78</t>
         </is>
       </c>
+      <c r="CK11" t="inlineStr">
+        <is>
+          <t>300069.SZ; 金利华电; 19.5; 20.0%; 87011.5; 94</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -24174,6 +24329,11 @@
           <t>300258.SZ; 精锻科技; 16.82; 12.3%; 44740.0; 105</t>
         </is>
       </c>
+      <c r="CK12" t="inlineStr">
+        <is>
+          <t>300631.SZ; 久吾高科; 24.58; 20.0%; 84133.0; 96</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -24614,6 +24774,11 @@
           <t>300328.SZ; 宜安科技; 12.79; 14.4%; 44430.0; 106</t>
         </is>
       </c>
+      <c r="CK13" t="inlineStr">
+        <is>
+          <t>300607.SZ; 拓斯达; 38.6; 2.1%; 79412.0; 103</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -25054,6 +25219,11 @@
           <t>301076.SZ; 新瀚新材; 42.5; 16.6%; 44017.5; 108</t>
         </is>
       </c>
+      <c r="CK14" t="inlineStr">
+        <is>
+          <t>300251.SZ; 光线传媒; 18.39; 0.5%; 76512.5; 106</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -25494,6 +25664,11 @@
           <t>300766.SZ; 每日互动; 40.93; 4.2%; 43875.5; 109</t>
         </is>
       </c>
+      <c r="CK15" t="inlineStr">
+        <is>
+          <t>300946.SZ; 恒而达; 84.44; 5.5%; 70476.0; 108</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -25934,6 +26109,11 @@
           <t>301301.SZ; 川宁生物; 13.69; -2.4%; 36995.0; 130</t>
         </is>
       </c>
+      <c r="CK16" t="inlineStr">
+        <is>
+          <t>300307.SZ; 慈星股份; 8.99; 3.5%; 64861.5; 116</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -26374,6 +26554,11 @@
           <t>688755.SH; 汉邦科技; 46.1; 102.5%; 36599.0; 131</t>
         </is>
       </c>
+      <c r="CK17" t="inlineStr">
+        <is>
+          <t>300004.SZ; 南风股份; 9.96; 11.9%; 63971.5; 118</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -26814,6 +26999,11 @@
           <t>300059.SZ; 东方财富; 21.53; -1.3%; 35133.0; 136</t>
         </is>
       </c>
+      <c r="CK18" t="inlineStr">
+        <is>
+          <t>300750.SZ; 宁德时代; 260; 0.2%; 62976.5; 119</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -27254,6 +27444,11 @@
           <t>300927.SZ; 江天化学; 30.69; 10.2%; 32864.0; 146</t>
         </is>
       </c>
+      <c r="CK19" t="inlineStr">
+        <is>
+          <t>301459.SZ; 丰茂股份; 65.75; 20.0%; 61666.5; 120</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -27694,6 +27889,11 @@
           <t>300695.SZ; 兆丰股份; 100.56; 13.2%; 32545.5; 150</t>
         </is>
       </c>
+      <c r="CK20" t="inlineStr">
+        <is>
+          <t>300132.SZ; 青松股份; 6.66; 12.3%; 61247.5; 121</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -28132,6 +28332,11 @@
       <c r="CJ21" t="inlineStr">
         <is>
           <t>300750.SZ; 宁德时代; 259.36; -0.3%; 32524.5; 151</t>
+        </is>
+      </c>
+      <c r="CK21" t="inlineStr">
+        <is>
+          <t>301089.SZ; 拓新药业; 38.3; 1.4%; 58151.5; 130</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update data with log
</commit_message>
<xml_diff>
--- a/excel/fupan_stocks_non_main.xlsx
+++ b/excel/fupan_stocks_non_main.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EL13"/>
+  <dimension ref="A1:EO13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1144,6 +1144,21 @@
           <t>2025年08月01日</t>
         </is>
       </c>
+      <c r="EM1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月04日</t>
+        </is>
+      </c>
+      <c r="EN1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月05日</t>
+        </is>
+      </c>
+      <c r="EO1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月06日</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -1589,6 +1604,21 @@
           <t>300289.SZ; 利德曼; 1;  09:30:36; 2天2板; 8.45;  09:25:00; 20.0%; 2; 重大重组+体外诊断+国企改革</t>
         </is>
       </c>
+      <c r="EM2" t="inlineStr">
+        <is>
+          <t>300486.SZ; 东杰智能; 2;  09:35:45; 2天2板; 16.99;  09:32:00; 20.0%; 2; 智能物流+机器人概念+实控人或变更+国企改革</t>
+        </is>
+      </c>
+      <c r="EN2" t="inlineStr">
+        <is>
+          <t>688585.SH; 上纬新材; 0;  14:56:15; 20天12板; 110.48;  14:56:15; 20.0%; 1; 智元机器人核心团队持股平台拟入主+风电材料</t>
+        </is>
+      </c>
+      <c r="EO2" t="inlineStr">
+        <is>
+          <t>301076.SZ; 新瀚新材; 1;  09:49:36; 2天2板; 44.58;  09:38:24; 20.0%; 2; DFBP（PEEK材料核心原料）+芳香族酮类</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -1839,6 +1869,21 @@
           <t>688189.SH; 南新制药; 2;  09:42:36; 2天2板; 17.14;  09:34:57; 20.0%; 2; 创新药+抗流感+国企改革</t>
         </is>
       </c>
+      <c r="EM3" t="inlineStr">
+        <is>
+          <t>688110.SH; 东芯股份; 1;  14:38:39; 5天3板; 68.88;  10:42:21; 20.0%; 1; 砺算科技+存储芯片+存算联一体化</t>
+        </is>
+      </c>
+      <c r="EN3" t="inlineStr">
+        <is>
+          <t>300486.SZ; 东杰智能; 7;  15:00:00; 3天3板; 20.39;  09:43:33; 20.0%; 3; 智能物流+机器人概念+实控人或变更+国企改革</t>
+        </is>
+      </c>
+      <c r="EO3" t="inlineStr">
+        <is>
+          <t>301357.SZ; 北方长龙; 19;  14:06:39; 3天2板; 157.9;  13:29:18; 20.0%; 1; 军工装备+非金属复合材料+无人机业务</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -1972,6 +2017,11 @@
       <c r="EI4" t="inlineStr">
         <is>
           <t>301038.SZ; 深水规院; 6;  14:45:57; 7天5板; 30.67;  14:37:15; 20.0%; 1; 水利+雅下水电概念+AI水科技+深圳国资</t>
+        </is>
+      </c>
+      <c r="EM4" t="inlineStr">
+        <is>
+          <t>300289.SZ; 利德曼; 11;  14:50:33; 3天3板; 10.14;  14:04:03; 20.0%; 3; 重大重组+体外诊断+国企改革</t>
         </is>
       </c>
     </row>
@@ -2161,7 +2211,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EL532"/>
+  <dimension ref="A1:EO532"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2873,6 +2923,21 @@
       <c r="EL1" s="1" t="inlineStr">
         <is>
           <t>2025年08月01日</t>
+        </is>
+      </c>
+      <c r="EM1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月04日</t>
+        </is>
+      </c>
+      <c r="EN1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月05日</t>
+        </is>
+      </c>
+      <c r="EO1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月06日</t>
         </is>
       </c>
     </row>
@@ -8272,7 +8337,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EL12"/>
+  <dimension ref="A1:EO12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8986,6 +9051,21 @@
           <t>2025年08月01日</t>
         </is>
       </c>
+      <c r="EM1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月04日</t>
+        </is>
+      </c>
+      <c r="EN1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月05日</t>
+        </is>
+      </c>
+      <c r="EO1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月06日</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -9651,6 +9731,16 @@
           <t>300350.SZ; 华鹏飞; 1;  09:35:00; 6.71; 曾涨停; 7.9%; 0.00H;  09:35:00</t>
         </is>
       </c>
+      <c r="EN2" t="inlineStr">
+        <is>
+          <t>300554.SZ; 三超新材; 1;  09:25:00; 25.8; 曾涨停; 7.1%; 0.02H;  09:25:00</t>
+        </is>
+      </c>
+      <c r="EO2" t="inlineStr">
+        <is>
+          <t>300329.SZ; 海伦钢琴; 1;  09:42:42; 12.44; 曾涨停; 3.2%; 0.04H;  09:42:42</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -10221,6 +10311,16 @@
           <t>688680.SH; 海优新材; 1;  10:09:49; 51.7; 曾涨停; 12.9%; 0.02H;  10:09:49</t>
         </is>
       </c>
+      <c r="EN3" t="inlineStr">
+        <is>
+          <t>301179.SZ; 泽宇智能; 2;  09:39:06; 17.05; 曾涨停; 14.0%; 0.62H;  09:39:06|| 10:18:00</t>
+        </is>
+      </c>
+      <c r="EO3" t="inlineStr">
+        <is>
+          <t>301397.SZ; 溯联股份; 1;  09:52:30; 36.21; 曾涨停; 13.8%; 0.03H;  09:52:30</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -10631,6 +10731,16 @@
           <t>301213.SZ; 观想科技; 1;  10:32:15; 67.99; 曾涨停; 12.8%; 0.03H;  10:32:15</t>
         </is>
       </c>
+      <c r="EN4" t="inlineStr">
+        <is>
+          <t>300455.SZ; 航天智装; 3;  09:46:00; 17.03; 曾涨停; 16.5%; 0.26H;  09:46:00|| 09:48:18|| 09:57:12</t>
+        </is>
+      </c>
+      <c r="EO4" t="inlineStr">
+        <is>
+          <t>688167.SH; 炬光科技; 1;  13:53:37; 100.01; 曾涨停; 16.2%; 0.00H;  13:53:37</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -10894,6 +11004,11 @@
       <c r="EL5" t="inlineStr">
         <is>
           <t>833266.BJ; 生物谷; 1;  10:59:31; 13.99; 曾涨停; 23.2%; 0.06H;  10:59:31</t>
+        </is>
+      </c>
+      <c r="EN5" t="inlineStr">
+        <is>
+          <t>300218.SZ; 安利股份; 1;  10:08:39; 19.22; 曾涨停; 12.1%; 0.32H;  10:08:39</t>
         </is>
       </c>
     </row>
@@ -11348,7 +11463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EL30"/>
+  <dimension ref="A1:EO30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12062,6 +12177,21 @@
           <t>2025年08月01日</t>
         </is>
       </c>
+      <c r="EM1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月04日</t>
+        </is>
+      </c>
+      <c r="EN1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月05日</t>
+        </is>
+      </c>
+      <c r="EO1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月06日</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -12767,6 +12897,21 @@
           <t>300500.SZ; 启迪设计; 0;  09:33:27; 首板涨停; 16.08;  09:33:27; 20.0%; 1; AI应用+智算中心+一季报增长</t>
         </is>
       </c>
+      <c r="EM2" t="inlineStr">
+        <is>
+          <t>301389.SZ; 隆扬电子; 0;  09:36:54; 首板涨停; 51.72;  09:36:54; 20.0%; 1; 复合铜箔+电磁屏蔽材料+消费电子+并购重组</t>
+        </is>
+      </c>
+      <c r="EN2" t="inlineStr">
+        <is>
+          <t>688659.SH; 元琛科技; 0;  09:38:28; 首板涨停; 11.53;  09:38:28; 20.0%; 1; PET铜箔+环保+AI环保岛+海外布局</t>
+        </is>
+      </c>
+      <c r="EO2" t="inlineStr">
+        <is>
+          <t>301117.SZ; 佳缘科技; 0;  09:36:57; 首板涨停; 35.72;  09:36:57; 20.0%; 1; 军工+医疗AI+SIP芯片+网络安全</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -13452,6 +13597,21 @@
           <t>688098.SH; 申联生物; 0;  09:48:24; 首板涨停; 8.48;  09:48:24; 19.9%; 1; 动物疫苗+多联多价疫苗+合作开发</t>
         </is>
       </c>
+      <c r="EM3" t="inlineStr">
+        <is>
+          <t>300696.SZ; 爱乐达; 3;  09:43:42; 首板涨停; 30.12;  09:32:42; 20.0%; 1; 军工+商业航天+大飞机+无人机</t>
+        </is>
+      </c>
+      <c r="EN3" t="inlineStr">
+        <is>
+          <t>300069.SZ; 金利华电; 0;  10:19:15; 首板涨停; 25.64;  10:19:15; 20.0%; 1; 玻璃绝缘子+航空航天+并购重组</t>
+        </is>
+      </c>
+      <c r="EO3" t="inlineStr">
+        <is>
+          <t>300572.SZ; 安车检测; 2;  10:14:48; 首板涨停; 31.21;  09:56:57; 20.0%; 1; 控制权变更+复牌+新能源汽车检测+机动车检测</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -14102,6 +14262,21 @@
           <t>300878.SZ; 维康药业; 0;  09:56:24; 首板涨停; 25.62;  09:56:24; 20.0%; 1; 黄甲软肝+创新药+中药</t>
         </is>
       </c>
+      <c r="EM4" t="inlineStr">
+        <is>
+          <t>688788.SH; 科思科技; 0;  10:16:25; 首板涨停; 72.73;  10:16:25; 20.0%; 1; 军工电子+无人机+AI应用</t>
+        </is>
+      </c>
+      <c r="EN4" t="inlineStr">
+        <is>
+          <t>300689.SZ; 澄天伟业; 0;  11:04:45; 首板涨停; 56.72;  11:04:45; 20.0%; 1; eSIM+智能卡+液冷+半导体封装材料</t>
+        </is>
+      </c>
+      <c r="EO4" t="inlineStr">
+        <is>
+          <t>688529.SH; 豪森智能; 0;  10:21:48; 首板涨停; 24.58;  10:21:48; 20.0%; 1; 人形机器人+智能制造</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -14687,6 +14862,21 @@
           <t>300724.SZ; 捷佳伟创; 7;  09:56:54; 首板涨停; 66.19;  09:31:15; 20.0%; 1; 业绩预增+光伏设备+半导体清洗</t>
         </is>
       </c>
+      <c r="EM5" t="inlineStr">
+        <is>
+          <t>688081.SH; 兴图新科; 0;  13:16:46; 首板涨停; 26.46;  13:16:46; 20.0%; 1; 军工+低空经济+AI技术</t>
+        </is>
+      </c>
+      <c r="EN5" t="inlineStr">
+        <is>
+          <t>301076.SZ; 新瀚新材; 6;  13:27:45; 首板涨停; 37.15;  11:11:27; 20.0%; 1; DFBP（PEEK材料核心原料）+芳香族酮类</t>
+        </is>
+      </c>
+      <c r="EO5" t="inlineStr">
+        <is>
+          <t>300600.SZ; 国瑞科技; 1;  10:53:18; 首板涨停; 20.7;  10:17:09; 20.0%; 1; 军工装备+商业航天+新能源船舶+国企改革</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -15222,6 +15412,21 @@
           <t>300329.SZ; 海伦钢琴; 0;  10:50:51; 首板涨停; 11;  10:50:51; 20.0%; 1; 智能电钢+乐器制造+三胎概念+控制权变更</t>
         </is>
       </c>
+      <c r="EM6" t="inlineStr">
+        <is>
+          <t>301357.SZ; 北方长龙; 0;  13:20:48; 首板涨停; 114.78;  13:20:48; 20.0%; 1; 军工装备+非金属复合材料+无人机业务</t>
+        </is>
+      </c>
+      <c r="EN6" t="inlineStr">
+        <is>
+          <t>300943.SZ; 春晖智控; 0;  13:29:36; 首板涨停; 18.62;  13:29:36; 20.0%; 1; 无人机+卫星导航+氢能源+汽车热管理</t>
+        </is>
+      </c>
+      <c r="EO6" t="inlineStr">
+        <is>
+          <t>300166.SZ; 东方国信; 0;  10:56:39; 首板涨停; 12.71;  10:56:39; 20.0%; 1; 华为昇思+智算中心+新型工业化+数字货币</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -15662,6 +15867,21 @@
           <t>688800.SH; 瑞可达; 8;  10:55:44; 首板涨停; 64.1;  10:07:35; 20.0%; 1; 人形机器人+连接器+业绩预增</t>
         </is>
       </c>
+      <c r="EM7" t="inlineStr">
+        <is>
+          <t>300965.SZ; 恒宇信通; 0;  13:23:30; 首板涨停; 76.09;  13:23:30; 20.0%; 1; 军工电子+直升机显控设备</t>
+        </is>
+      </c>
+      <c r="EN7" t="inlineStr">
+        <is>
+          <t>300916.SZ; 朗特智能; 2;  14:34:42; 首板涨停; 42.73;  13:20:03; 20.0%; 1; 机器人概念+智能控制器+消费电子</t>
+        </is>
+      </c>
+      <c r="EO7" t="inlineStr">
+        <is>
+          <t>301616.SZ; 浙江华业; 7;  11:15:12; 首板涨停; 52.39;  10:46:39; 20.0%; 1; 注塑机+机器人概念+一季报增长</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -16042,6 +16262,21 @@
           <t>300486.SZ; 东杰智能; 0;  13:06:24; 首板涨停; 14.16;  13:06:24; 20.0%; 1; 智能物流+机器人概念+实控人或变更+国企改革</t>
         </is>
       </c>
+      <c r="EM8" t="inlineStr">
+        <is>
+          <t>300199.SZ; 翰宇药业; 1;  14:04:45; 首板涨停; 24.32;  13:27:03; 20.0%; 1; RWA+减重药+多肽药物+中报预增</t>
+        </is>
+      </c>
+      <c r="EN8" t="inlineStr">
+        <is>
+          <t>300960.SZ; 通业科技; 0;  14:40:03; 首板涨停; 33.92;  14:40:03; 20.0%; 1; 轨道交通+电机+海外拓展+高铁概念</t>
+        </is>
+      </c>
+      <c r="EO8" t="inlineStr">
+        <is>
+          <t>301069.SZ; 凯盛新材; 0;  11:20:09; 首板涨停; 21.56;  11:20:09; 20.0%; 1; PEEK材料+精细化工+一季报增长</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -16327,6 +16562,16 @@
           <t>300858.SZ; 科拓生物; 2;  14:51:27; 首板涨停; 20.4;  13:57:15; 20.0%; 1; 益生菌新药+幽门螺杆菌概念+宠物经济</t>
         </is>
       </c>
+      <c r="EM9" t="inlineStr">
+        <is>
+          <t>300830.SZ; 金现代; 0;  14:20:36; 首板涨停; 13.58;  14:20:36; 20.0%; 1; 低代码平台+实验室管理系统+国家电网+AI应用</t>
+        </is>
+      </c>
+      <c r="EO9" t="inlineStr">
+        <is>
+          <t>836247.BJ; 华密新材; 0;  11:21:58; 首板涨停; 30.84;  11:21:58; 30.0%; 1; 机器人皮肤+特种橡胶材料+军工+新能源汽车</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -16547,6 +16792,16 @@
           <t>300617.SZ; 安靠智电; 4;  10:16:24; 首板涨停; 36.73;  09:59:06; 20.0%; 1; 特高压+GIL+数据中心</t>
         </is>
       </c>
+      <c r="EM10" t="inlineStr">
+        <is>
+          <t>688265.SH; 南模生物; 3;  14:22:09; 首板涨停; 43.73;  14:08:45; 20.0%; 1; 基因修饰动物模型+医疗服务</t>
+        </is>
+      </c>
+      <c r="EO10" t="inlineStr">
+        <is>
+          <t>300731.SZ; 科创新源; 13;  13:15:57; 首板涨停; 47.12;  09:43:42; 20.0%; 1; 液冷服务器+新能源汽车液冷板+热管理</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -16727,6 +16982,16 @@
           <t>300808.SZ; 久量股份; 0;  10:16:30; 首板涨停; 35.94;  10:16:30; 20.0%; 1; LED照明+一带一路+国企改革</t>
         </is>
       </c>
+      <c r="EM11" t="inlineStr">
+        <is>
+          <t>300584.SZ; 海辰药业; 0;  14:23:21; 首板涨停; 41.27;  14:23:21; 20.0%; 1; 固态电池+创新药+一季报增长</t>
+        </is>
+      </c>
+      <c r="EO11" t="inlineStr">
+        <is>
+          <t>300875.SZ; 捷强装备; 0;  13:53:18; 首板涨停; 58.06;  13:53:18; 20.0%; 1; 军工装备+核生化安全+一季报好转</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -16857,6 +17122,11 @@
           <t>300722.SZ; 新余国科; 0;  10:49:33; 首板涨停; 41.05;  10:49:33; 20.0%; 1; 火工品+军工+国企</t>
         </is>
       </c>
+      <c r="EO12" t="inlineStr">
+        <is>
+          <t>688039.SH; 当虹科技; 0;  13:58:25; 首板涨停; 58.56;  13:58:25; 20.0%; 1; 机器人系统首发+AI视频技术+华为昇腾</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -16952,6 +17222,11 @@
           <t>301161.SZ; 唯万密封; 1;  13:08:03; 首板涨停; 29.59;  13:05:27; 20.0%; 1; 工程机械+股权收购+一季报增长</t>
         </is>
       </c>
+      <c r="EO13" t="inlineStr">
+        <is>
+          <t>300906.SZ; 日月明; 0;  14:19:45; 首板涨停; 35.66;  14:19:45; 20.0%; 1; 高铁+专精特新+年报增长</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -17032,6 +17307,11 @@
           <t>300718.SZ; 长盛轴承; 8;  14:09:15; 首板涨停; 95.28;  09:44:00; 20.0%; 1; 机器人+自润滑轴承+业绩增长</t>
         </is>
       </c>
+      <c r="EO14" t="inlineStr">
+        <is>
+          <t>300885.SZ; 海昌新材; 0;  14:27:42; 首板涨停; 28.86;  14:27:42; 20.0%; 1; 人形机器人+粉末冶金+一季报增长</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -17105,6 +17385,11 @@
       <c r="EC15" t="inlineStr">
         <is>
           <t>873706.BJ; 铁拓机械; 1;  14:22:59; 首板涨停; 24.01;  14:17:41; 30.0%; 1; 沥青混合料搅拌设备+海外销售增长+俄罗斯市场</t>
+        </is>
+      </c>
+      <c r="EO15" t="inlineStr">
+        <is>
+          <t>688711.SH; 宏微科技; 0;  14:35:14; 首板涨停; 31.22;  14:35:14; 20.0%; 1; 机器人探索+SiC增长+可控核聚变</t>
         </is>
       </c>
     </row>
@@ -17469,7 +17754,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EL178"/>
+  <dimension ref="A1:EO178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18183,6 +18468,21 @@
           <t>2025年08月01日</t>
         </is>
       </c>
+      <c r="EM1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月04日</t>
+        </is>
+      </c>
+      <c r="EN1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月05日</t>
+        </is>
+      </c>
+      <c r="EO1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月06日</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -18863,6 +19163,21 @@
           <t>300486.SZ; 东杰智能; 2.5%; 23.1%; 14.16; 20.0%; 价升量涨||阳线||放量</t>
         </is>
       </c>
+      <c r="EM2" t="inlineStr">
+        <is>
+          <t>300966.SZ; 共同药业; 6.3%; 13.3%; 28.33; 6.2%; 阳线||放量||价升量缩</t>
+        </is>
+      </c>
+      <c r="EN2" t="inlineStr">
+        <is>
+          <t>300731.SZ; 科创新源; 5.5%; 12.6%; 39.27; 6.4%; 价升量涨||强中选强||阳线</t>
+        </is>
+      </c>
+      <c r="EO2" t="inlineStr">
+        <is>
+          <t>836247.BJ; 华密新材; 3.0%; 33.9%; 30.84; 30.0%; 价升量涨||强中选强||阳线</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -19503,6 +19818,21 @@
           <t>300519.SZ; 新光药业; 2.0%; 15.0%; 19.8; 12.8%; 价升量涨||阳线||放量</t>
         </is>
       </c>
+      <c r="EM3" t="inlineStr">
+        <is>
+          <t>301357.SZ; 北方长龙; 3.8%; 24.7%; 114.78; 20.0%; 强中选强||阳线||放量</t>
+        </is>
+      </c>
+      <c r="EN3" t="inlineStr">
+        <is>
+          <t>301678.SZ; 新恒汇; 1.8%; 18.4%; 91.81; 16.2%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
+      <c r="EO3" t="inlineStr">
+        <is>
+          <t>300644.SZ; 南京聚隆; 1.8%; 18.1%; 41.9; 15.9%; 价升量涨||强中选强||阳线</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -20088,6 +20418,21 @@
           <t>300858.SZ; 科拓生物; 1.0%; 21.2%; 20.4; 20.0%; 价升量涨||阳线||放量</t>
         </is>
       </c>
+      <c r="EM4" t="inlineStr">
+        <is>
+          <t>300591.SZ; 万里马; 2.3%; 15.1%; 12.6; 12.4%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
+      <c r="EN4" t="inlineStr">
+        <is>
+          <t>300732.SZ; 设研院; 1.4%; 13.0%; 11.58; 11.3%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
+      <c r="EO4" t="inlineStr">
+        <is>
+          <t>300581.SZ; 晨曦航空; 1.7%; 13.5%; 24.38; 11.6%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -20603,6 +20948,21 @@
           <t>301678.SZ; 新恒汇; 0.6%; 15.1%; 76.65; 14.4%; 价升量涨||阳线||放量</t>
         </is>
       </c>
+      <c r="EM5" t="inlineStr">
+        <is>
+          <t>832885.BJ; 星辰科技; 2.1%; 18.4%; 27.37; 15.9%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
+      <c r="EN5" t="inlineStr">
+        <is>
+          <t>301357.SZ; 北方长龙; 0.9%; 15.7%; 131.58; 14.6%; 价升量涨||强中选强||阳线</t>
+        </is>
+      </c>
+      <c r="EO5" t="inlineStr">
+        <is>
+          <t>832469.BJ; 富恒新材; 1.5%; 17.8%; 17.44; 16.0%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -21068,6 +21428,16 @@
           <t>301213.SZ; 观想科技; 0.5%; 13.3%; 67.99; 12.8%; 价升量涨||阳线||放量</t>
         </is>
       </c>
+      <c r="EM6" t="inlineStr">
+        <is>
+          <t>688258.SH; 卓易信息; 1.8%; 14.1%; 75.43; 12.1%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
+      <c r="EO6" t="inlineStr">
+        <is>
+          <t>300885.SZ; 海昌新材; 1.5%; 21.8%; 28.86; 20.0%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -21498,6 +21868,16 @@
           <t>301316.SZ; 慧博云通; 0.0%; 13.3%; 47.15; 13.3%; 价升量涨||阳线||放量</t>
         </is>
       </c>
+      <c r="EM7" t="inlineStr">
+        <is>
+          <t>300965.SZ; 恒宇信通; 1.4%; 21.7%; 76.09; 20.0%; 价升量涨||强中选强||阳线</t>
+        </is>
+      </c>
+      <c r="EO7" t="inlineStr">
+        <is>
+          <t>301357.SZ; 北方长龙; 1.2%; 21.5%; 157.9; 20.0%; 强中选强||阳线||放量</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -21858,6 +22238,16 @@
           <t>300368.SZ; 汇金股份; 0.7%; 16.0%; 11.61; 15.2%; 价升量涨||阳线||放量</t>
         </is>
       </c>
+      <c r="EM8" t="inlineStr">
+        <is>
+          <t>688011.SH; 新光光电; 1.0%; 14.7%; 49.06; 13.5%; 阳线||放量||价升量缩</t>
+        </is>
+      </c>
+      <c r="EO8" t="inlineStr">
+        <is>
+          <t>300875.SZ; 捷强装备; 1.2%; 21.5%; 58.06; 20.0%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -22153,6 +22543,16 @@
           <t>688303.SH; 大全能源; 0.5%; 12.3%; 26.5; 11.7%; 价升量涨||强中选强||阳线</t>
         </is>
       </c>
+      <c r="EM9" t="inlineStr">
+        <is>
+          <t>688376.SH; 美埃科技; 0.9%; 12.4%; 48.35; 11.4%; 价升量涨||强中选强||阳线</t>
+        </is>
+      </c>
+      <c r="EO9" t="inlineStr">
+        <is>
+          <t>301117.SZ; 佳缘科技; 1.0%; 21.2%; 35.72; 20.0%; 阳线||放量||价升量缩</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -22408,6 +22808,16 @@
           <t>688073.SH; 毕得医药; 0.0%; 13.0%; 58.02; 13.0%; 价升量涨||阳线||放量</t>
         </is>
       </c>
+      <c r="EM10" t="inlineStr">
+        <is>
+          <t>301161.SZ; 唯万密封; 0.7%; 13.2%; 31.19; 12.4%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
+      <c r="EO10" t="inlineStr">
+        <is>
+          <t>688711.SH; 宏微科技; 0.8%; 21.0%; 31.22; 20.0%; 价升量涨||强中选强||阳线</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -22623,6 +23033,16 @@
           <t>920098.BJ; 科隆新材; 0.4%; 13.2%; 38.5; 12.7%; 价升量涨||阳线||放量</t>
         </is>
       </c>
+      <c r="EM11" t="inlineStr">
+        <is>
+          <t>300436.SZ; 广生堂; 0.6%; 18.9%; 120.9; 18.2%; 强中选强||阳线||缩量</t>
+        </is>
+      </c>
+      <c r="EO11" t="inlineStr">
+        <is>
+          <t>300906.SZ; 日月明; 0.3%; 20.3%; 35.66; 20.0%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -22773,6 +23193,16 @@
           <t>688318.SH; 财富趋势; 0.4%; 18.3%; 124.01; 17.8%; 价升量涨||阳线||放量</t>
         </is>
       </c>
+      <c r="EM12" t="inlineStr">
+        <is>
+          <t>301529.SZ; 福赛科技; 0.5%; 14.9%; 70.31; 14.3%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
+      <c r="EO12" t="inlineStr">
+        <is>
+          <t>688660.SH; 电气风电; 0.1%; 15.2%; 16.35; 15.1%; 价升量涨||强中选强||阳线</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -22903,6 +23333,16 @@
           <t>300600.SZ; 国瑞科技; 0.2%; 20.3%; 11.27; 20.0%; 价升量涨||阳线||放量</t>
         </is>
       </c>
+      <c r="EM13" t="inlineStr">
+        <is>
+          <t>688163.SH; 赛伦生物; 0.5%; 12.4%; 27.37; 11.9%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
+      <c r="EO13" t="inlineStr">
+        <is>
+          <t>300572.SZ; 安车检测; 0.0%; 20.0%; 31.21; 20.0%; 价升量涨||强中选强||阳线</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -23008,6 +23448,16 @@
           <t>688282.SH; 理工导航; 0.1%; 13.1%; 47.3; 13.0%; 价升量涨||阳线||放量</t>
         </is>
       </c>
+      <c r="EM14" t="inlineStr">
+        <is>
+          <t>688059.SH; 华锐精密; 0.4%; 14.2%; 62.38; 13.8%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
+      <c r="EO14" t="inlineStr">
+        <is>
+          <t>301397.SZ; 溯联股份; 0.0%; 13.9%; 36.21; 13.8%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -23093,6 +23543,11 @@
           <t>301292.SZ; 海科新源; 0.4%; 13.9%; 26.68; 13.4%; 价升量涨||强中选强||阳线</t>
         </is>
       </c>
+      <c r="EM15" t="inlineStr">
+        <is>
+          <t>300696.SZ; 爱乐达; 0.4%; 20.4%; 30.12; 20.0%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -23168,6 +23623,11 @@
           <t>301003.SZ; 江苏博云; 0.1%; 13.0%; 31.08; 12.9%; 价升量涨||阳线||放量</t>
         </is>
       </c>
+      <c r="EM16" t="inlineStr">
+        <is>
+          <t>300648.SZ; 星云股份; 0.1%; 15.0%; 49.9; 14.9%; 价升量涨||阳线||放量</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -23241,6 +23701,11 @@
       <c r="DI17" t="inlineStr">
         <is>
           <t>300773.SZ; 拉卡拉; 0.0%; 13.1%; 31.9; 13.0%; 价升量涨||强中选强||阳线</t>
+        </is>
+      </c>
+      <c r="EM17" t="inlineStr">
+        <is>
+          <t>300199.SZ; 翰宇药业; 0.0%; 20.0%; 24.32; 20.0%; 价升量涨||阳线||放量</t>
         </is>
       </c>
     </row>
@@ -25260,7 +25725,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EL21"/>
+  <dimension ref="A1:EO21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25974,6 +26439,21 @@
           <t>2025年08月01日</t>
         </is>
       </c>
+      <c r="EM1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月04日</t>
+        </is>
+      </c>
+      <c r="EN1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月05日</t>
+        </is>
+      </c>
+      <c r="EO1" s="1" t="inlineStr">
+        <is>
+          <t>2025年08月06日</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -26684,6 +27164,21 @@
           <t>300527.SZ; ST应急; 10.01; -20.0%; 255716.0; 3</t>
         </is>
       </c>
+      <c r="EM2" t="inlineStr">
+        <is>
+          <t>300199.SZ; 翰宇药业; 24.32; 20.0%; 364089.5; 4</t>
+        </is>
+      </c>
+      <c r="EN2" t="inlineStr">
+        <is>
+          <t>688585.SH; 上纬新材; 110.48; 20.0%; 981725.5; 1</t>
+        </is>
+      </c>
+      <c r="EO2" t="inlineStr">
+        <is>
+          <t>688585.SH; 上纬新材; 88.38; -20.0%; 423971.0; 4</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -27394,6 +27889,21 @@
           <t>300724.SZ; 捷佳伟创; 66.19; 20.0%; 155247.5; 11</t>
         </is>
       </c>
+      <c r="EM3" t="inlineStr">
+        <is>
+          <t>688585.SH; 上纬新材; 92.07; 0.0%; 330394.0; 5</t>
+        </is>
+      </c>
+      <c r="EN3" t="inlineStr">
+        <is>
+          <t>300486.SZ; 东杰智能; 20.39; 20.0%; 290850.5; 6</t>
+        </is>
+      </c>
+      <c r="EO3" t="inlineStr">
+        <is>
+          <t>301357.SZ; 北方长龙; 157.9; 20.0%; 248977.5; 13</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -28104,6 +28614,21 @@
           <t>300486.SZ; 东杰智能; 14.16; 20.0%; 121207.5; 16</t>
         </is>
       </c>
+      <c r="EM4" t="inlineStr">
+        <is>
+          <t>301357.SZ; 北方长龙; 114.78; 20.0%; 185856.0; 13</t>
+        </is>
+      </c>
+      <c r="EN4" t="inlineStr">
+        <is>
+          <t>300199.SZ; 翰宇药业; 25.69; 5.6%; 132108.5; 26</t>
+        </is>
+      </c>
+      <c r="EO4" t="inlineStr">
+        <is>
+          <t>300166.SZ; 东方国信; 12.71; 20.0%; 203824.5; 22</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -28814,6 +29339,21 @@
           <t>300378.SZ; 鼎捷数智; 60.99; 16.1%; 121109.0; 17</t>
         </is>
       </c>
+      <c r="EM5" t="inlineStr">
+        <is>
+          <t>300289.SZ; 利德曼; 10.14; 20.0%; 169268.0; 19</t>
+        </is>
+      </c>
+      <c r="EN5" t="inlineStr">
+        <is>
+          <t>301678.SZ; 新恒汇; 91.81; 16.2%; 129547.0; 28</t>
+        </is>
+      </c>
+      <c r="EO5" t="inlineStr">
+        <is>
+          <t>300024.SZ; 机器人; 20.09; 14.7%; 166145.0; 27</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -29524,6 +30064,21 @@
           <t>300308.SZ; 中际旭创; 210.63; -3.2%; 112241.5; 21</t>
         </is>
       </c>
+      <c r="EM6" t="inlineStr">
+        <is>
+          <t>300830.SZ; 金现代; 13.58; 20.0%; 157758.0; 22</t>
+        </is>
+      </c>
+      <c r="EN6" t="inlineStr">
+        <is>
+          <t>301357.SZ; 北方长龙; 131.58; 14.6%; 121979.5; 34</t>
+        </is>
+      </c>
+      <c r="EO6" t="inlineStr">
+        <is>
+          <t>300885.SZ; 海昌新材; 28.86; 20.0%; 160842.0; 28</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -30234,6 +30789,21 @@
           <t>300289.SZ; 利德曼; 8.45; 20.0%; 104241.0; 23</t>
         </is>
       </c>
+      <c r="EM7" t="inlineStr">
+        <is>
+          <t>300486.SZ; 东杰智能; 16.99; 20.0%; 150839.0; 24</t>
+        </is>
+      </c>
+      <c r="EN7" t="inlineStr">
+        <is>
+          <t>301076.SZ; 新瀚新材; 37.15; 20.0%; 114356.0; 38</t>
+        </is>
+      </c>
+      <c r="EO7" t="inlineStr">
+        <is>
+          <t>301491.SZ; 汉桑科技; 82.89; 186.7%; 153233.5; 31</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -30944,6 +31514,21 @@
           <t>300624.SZ; 万兴科技; 89.6; 11.0%; 94593.0; 32</t>
         </is>
       </c>
+      <c r="EM8" t="inlineStr">
+        <is>
+          <t>300584.SZ; 海辰药业; 41.27; 20.0%; 147603.5; 26</t>
+        </is>
+      </c>
+      <c r="EN8" t="inlineStr">
+        <is>
+          <t>688041.SH; 海光信息; 142.46; -0.1%; 92967.0; 50</t>
+        </is>
+      </c>
+      <c r="EO8" t="inlineStr">
+        <is>
+          <t>301076.SZ; 新瀚新材; 44.58; 20.0%; 150305.0; 33</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -31654,6 +32239,21 @@
           <t>301171.SZ; 易点天下; 35.3; 5.2%; 83763.0; 42</t>
         </is>
       </c>
+      <c r="EM9" t="inlineStr">
+        <is>
+          <t>300696.SZ; 爱乐达; 30.12; 20.0%; 140905.0; 30</t>
+        </is>
+      </c>
+      <c r="EN9" t="inlineStr">
+        <is>
+          <t>300689.SZ; 澄天伟业; 56.72; 20.0%; 76871.5; 66</t>
+        </is>
+      </c>
+      <c r="EO9" t="inlineStr">
+        <is>
+          <t>300875.SZ; 捷强装备; 58.06; 20.0%; 147225.0; 34</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -32364,6 +32964,21 @@
           <t>300500.SZ; 启迪设计; 16.08; 20.0%; 79519.0; 47</t>
         </is>
       </c>
+      <c r="EM10" t="inlineStr">
+        <is>
+          <t>300436.SZ; 广生堂; 120.9; 18.2%; 135933.5; 32</t>
+        </is>
+      </c>
+      <c r="EN10" t="inlineStr">
+        <is>
+          <t>300916.SZ; 朗特智能; 42.73; 20.0%; 75702.5; 67</t>
+        </is>
+      </c>
+      <c r="EO10" t="inlineStr">
+        <is>
+          <t>300486.SZ; 东杰智能; 17.04; -16.4%; 125693.5; 41</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -33074,6 +33689,21 @@
           <t>300878.SZ; 维康药业; 25.62; 20.0%; 69560.5; 60</t>
         </is>
       </c>
+      <c r="EM11" t="inlineStr">
+        <is>
+          <t>688110.SH; 东芯股份; 68.88; 20.0%; 116203.0; 45</t>
+        </is>
+      </c>
+      <c r="EN11" t="inlineStr">
+        <is>
+          <t>300436.SZ; 广生堂; 123.55; 2.2%; 75335.5; 70</t>
+        </is>
+      </c>
+      <c r="EO11" t="inlineStr">
+        <is>
+          <t>300591.SZ; 万里马; 14; 11.8%; 119853.0; 46</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -33784,6 +34414,21 @@
           <t>688585.SH; 上纬新材; 92.07; 0.0%; 62706.5; 69</t>
         </is>
       </c>
+      <c r="EM12" t="inlineStr">
+        <is>
+          <t>300527.SZ; ST应急; 9.43; -5.8%; 102406.0; 52</t>
+        </is>
+      </c>
+      <c r="EN12" t="inlineStr">
+        <is>
+          <t>300289.SZ; 利德曼; 9.19; -9.4%; 73815.0; 73</t>
+        </is>
+      </c>
+      <c r="EO12" t="inlineStr">
+        <is>
+          <t>836247.BJ; 华密新材; 30.84; 30.0%; 116882.0; 49</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -34494,6 +35139,21 @@
           <t>300436.SZ; 广生堂; 102.3; -10.7%; 62622.0; 70</t>
         </is>
       </c>
+      <c r="EM13" t="inlineStr">
+        <is>
+          <t>300528.SZ; 幸福蓝海; 18.93; -11.3%; 101465.5; 53</t>
+        </is>
+      </c>
+      <c r="EN13" t="inlineStr">
+        <is>
+          <t>300322.SZ; 硕贝德; 20.64; 6.4%; 72975.0; 75</t>
+        </is>
+      </c>
+      <c r="EO13" t="inlineStr">
+        <is>
+          <t>300229.SZ; 拓尔思; 26.32; 9.0%; 110686.5; 52</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -35204,6 +35864,21 @@
           <t>300528.SZ; 幸福蓝海; 21.35; -8.1%; 60761.5; 75</t>
         </is>
       </c>
+      <c r="EM14" t="inlineStr">
+        <is>
+          <t>300378.SZ; 鼎捷数智; 65.02; 6.6%; 99012.0; 56</t>
+        </is>
+      </c>
+      <c r="EN14" t="inlineStr">
+        <is>
+          <t>300455.SZ; 航天智装; 17.03; 16.5%; 71951.5; 78</t>
+        </is>
+      </c>
+      <c r="EO14" t="inlineStr">
+        <is>
+          <t>300600.SZ; 国瑞科技; 20.7; 20.0%; 99081.0; 59</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -35914,6 +36589,21 @@
           <t>300657.SZ; 弘信电子; 29.27; -1.1%; 58267.5; 79</t>
         </is>
       </c>
+      <c r="EM15" t="inlineStr">
+        <is>
+          <t>301389.SZ; 隆扬电子; 51.72; 20.0%; 89498.5; 66</t>
+        </is>
+      </c>
+      <c r="EN15" t="inlineStr">
+        <is>
+          <t>300732.SZ; 设研院; 11.58; 11.3%; 69818.5; 83</t>
+        </is>
+      </c>
+      <c r="EO15" t="inlineStr">
+        <is>
+          <t>300718.SZ; 长盛轴承; 102; 7.7%; 96497.5; 62</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -36624,6 +37314,21 @@
           <t>300182.SZ; 捷成股份; 6.11; 6.4%; 55458.5; 86</t>
         </is>
       </c>
+      <c r="EM16" t="inlineStr">
+        <is>
+          <t>300718.SZ; 长盛轴承; 93.82; 8.9%; 80384.0; 77</t>
+        </is>
+      </c>
+      <c r="EN16" t="inlineStr">
+        <is>
+          <t>300696.SZ; 爱乐达; 32.17; 6.8%; 69393.5; 85</t>
+        </is>
+      </c>
+      <c r="EO16" t="inlineStr">
+        <is>
+          <t>300199.SZ; 翰宇药业; 23.4; -8.9%; 93553.5; 64</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -37334,6 +38039,21 @@
           <t>300476.SZ; 胜宏科技; 191.35; -0.4%; 55251.5; 87</t>
         </is>
       </c>
+      <c r="EM17" t="inlineStr">
+        <is>
+          <t>300965.SZ; 恒宇信通; 76.09; 20.0%; 75127.5; 83</t>
+        </is>
+      </c>
+      <c r="EN17" t="inlineStr">
+        <is>
+          <t>300943.SZ; 春晖智控; 18.62; 20.0%; 68863.5; 86</t>
+        </is>
+      </c>
+      <c r="EO17" t="inlineStr">
+        <is>
+          <t>688529.SH; 豪森智能; 24.58; 20.0%; 91803.0; 66</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -38044,6 +38764,21 @@
           <t>300858.SZ; 科拓生物; 20.4; 20.0%; 55052.5; 88</t>
         </is>
       </c>
+      <c r="EM18" t="inlineStr">
+        <is>
+          <t>300591.SZ; 万里马; 12.6; 12.4%; 74989.5; 84</t>
+        </is>
+      </c>
+      <c r="EN18" t="inlineStr">
+        <is>
+          <t>300706.SZ; 阿石创; 38.46; 10.2%; 67687.0; 87</t>
+        </is>
+      </c>
+      <c r="EO18" t="inlineStr">
+        <is>
+          <t>301117.SZ; 佳缘科技; 35.72; 20.0%; 90472.5; 67</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -38754,6 +39489,21 @@
           <t>300502.SZ; 新易盛; 183.12; -3.2%; 54504.0; 90</t>
         </is>
       </c>
+      <c r="EM19" t="inlineStr">
+        <is>
+          <t>300251.SZ; 光线传媒; 20.9; 3.8%; 63724.5; 101</t>
+        </is>
+      </c>
+      <c r="EN19" t="inlineStr">
+        <is>
+          <t>300548.SZ; 长芯博创; 95.4; 13.4%; 66859.0; 91</t>
+        </is>
+      </c>
+      <c r="EO19" t="inlineStr">
+        <is>
+          <t>300830.SZ; 金现代; 13.7; 7.4%; 89226.0; 68</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -39464,6 +40214,21 @@
           <t>300058.SZ; 蓝色光标; 7.18; 3.3%; 51571.5; 95</t>
         </is>
       </c>
+      <c r="EM20" t="inlineStr">
+        <is>
+          <t>688788.SH; 科思科技; 72.73; 20.0%; 56127.5; 115</t>
+        </is>
+      </c>
+      <c r="EN20" t="inlineStr">
+        <is>
+          <t>301200.SZ; 大族数控; 83.5; 14.2%; 66659.0; 93</t>
+        </is>
+      </c>
+      <c r="EO20" t="inlineStr">
+        <is>
+          <t>301069.SZ; 凯盛新材; 21.56; 20.0%; 89028.0; 69</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -40172,6 +40937,21 @@
       <c r="EL21" t="inlineStr">
         <is>
           <t>300170.SZ; 汉得信息; 19.96; 5.7%; 50436.0; 100</t>
+        </is>
+      </c>
+      <c r="EM21" t="inlineStr">
+        <is>
+          <t>300007.SZ; 汉威科技; 46.89; 8.2%; 55258.0; 118</t>
+        </is>
+      </c>
+      <c r="EN21" t="inlineStr">
+        <is>
+          <t>300871.SZ; 回盛生物; 24.82; 1.8%; 66463.0; 94</t>
+        </is>
+      </c>
+      <c r="EO21" t="inlineStr">
+        <is>
+          <t>300731.SZ; 科创新源; 47.12; 20.0%; 88189.0; 71</t>
         </is>
       </c>
     </row>

</xml_diff>